<commit_message>
QDS Ver 0.1.6 : - use select as image path - the image fliter need optimization
</commit_message>
<xml_diff>
--- a/database/盈虧問題v2.xlsx
+++ b/database/盈虧問題v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Question DataBase System\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89726044-7272-43AC-A125-8565240E0AF8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3774C0DA-C860-4EA3-8B23-854676DBAD02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27027,7 +27027,7 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>database\\數學\\應用題\\典型應用題\\燕尾定理\\基本題\\1.png database\\數學\\應用題\\典型應用題\\燕尾定理\\基本題\\2.png</t>
+    <t>1.png 2.png</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -33160,7 +33160,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="49.5">
+    <row r="212" spans="1:8" ht="16.5">
       <c r="A212" s="6" t="s">
         <v>190</v>
       </c>
@@ -33189,7 +33189,7 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <oleObjects>

</xml_diff>

<commit_message>
QDS Ver 0.1.7 : - Add a script to fetch image from word (under database) - The part of inserting image almost finish - Finish "Dovetail theorem" problem *To see more detail, please read "Update and Problem.txt"
</commit_message>
<xml_diff>
--- a/database/盈虧問題v2.xlsx
+++ b/database/盈虧問題v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Question DataBase System\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3774C0DA-C860-4EA3-8B23-854676DBAD02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDFED02-F7CE-4F09-9F39-F4AD9E9C414A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3285" yWindow="1830" windowWidth="10185" windowHeight="9795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="300">
   <si>
     <r>
       <rPr>
@@ -27027,7 +27027,271 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>1.png 2.png</t>
+    <t>如圖，△ABC中，若3BD ＝2CD ，則△ABF面積：△ACF面積的比值＝【2/3】</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">右圖的大三角形被分成5個小三角形，其中4個的面積已經標在圖中，那麼，陰影三角形的面積＝【2】
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.jpg</t>
+  </si>
+  <si>
+    <t>3.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>一外一內比1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>一外一內比2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">在△ABC中，BD＝2DC，AE＝ED。已知△ABC的面積是5 cm2。求陰影部份的面積 ＝【2】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.jpg</t>
+  </si>
+  <si>
+    <t>12.jpg</t>
+  </si>
+  <si>
+    <t>13.jpg</t>
+  </si>
+  <si>
+    <t>14.jpg</t>
+  </si>
+  <si>
+    <t>15.jpg</t>
+  </si>
+  <si>
+    <t>16.jpg</t>
+  </si>
+  <si>
+    <t>19.jpg</t>
+  </si>
+  <si>
+    <t>21.jpg</t>
+  </si>
+  <si>
+    <t>23.jpg</t>
+  </si>
+  <si>
+    <t>24.jpg</t>
+  </si>
+  <si>
+    <t>25.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">如圖所示，AE＝ED，BC＝3BD，△ABC面積是30 cm2。求：陰影部分的面積＝【12】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">在△ABC中，BD：DC＝2：3，E是AD的中點。求：陰影部份的面積是△ABC的幾分之幾：【3/8 】
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>若 BD：CD ＝2：5， AE：DE ＝1：4，則△ABE面積：△CDE面積＝【 1：10 】</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如圖，在△ABC中，DC＝3BD，AE＝ED。若△ABC的面積是1，則：陰影部份的面積＝【 3/7】
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>5_1.jpg 5_2.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>如圖，在△ABC中，BE：EC＝3：1，D是AE的中點，那麼AF：FC＝【3：4】</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>6_1.jpg 6_2.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">△ABC中， AD：DC ＝1：3，E為BD 之中點，AE 之延長線BC交 於F，則BF：FC ＝【 1：4 】
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> BD：CD ＝4：3， AE：ED ＝3：2，則△ABD　面積：△ABC　面積＝【 4：7 】；△ABE　面積：△ABC　面積＝【　12：35　】
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">△ABC中， AE：ED ＝2：1， BD：CD ＝5：3。若△AEC的面積為18cm2，則： △ABC的面積＝【72】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">△ABC中BC＝4CD， E是AD的中點。已知△ABC的面積是112 cm2，求：四邊形CDEF的面積＝【22】cm2
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>10_1.jpg 10_2.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">D是BC的中點，E是AD的中點。已知△ABC的面積是36 cm2。求：四邊形CDEF的面積＝【15】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">D是BC上的一點，BD＝3DC，E是AD上的一點，AE＝ED。那麼四邊形CDEF的面積是ABC面積的幾分之幾:【 11/56】
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如圖，已知△ABD的面積為72cm2，且DC＝ 1/2BD，AE＝ED，連接BE並延長，交AC於F。求：四邊形CDEF的面積＝【28.8】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如圖所示，AE＝ED，DC＝ BD，△ABC面積＝21 cm2。求：陰影部分的面積＝【9】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如圖，△ABC的面積為15cm2，D是BC邊上的一點，BD＝2DC，E是AD上的一點，AE＝ED，連接BE並延長，交AC於點F。求：圖中四邊形CDEF的面積【4】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如下圖，在△ABC中，BD＝2DC，AE＝ED，已知三角形ABC的面積是5cm2，求：陰影部份的面積是【2】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>已知S△ABC＝1，AE＝ED，BD＝ 2/3BC，求：陰影部分的面積＝【2/5 】</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>17_1.jpg 17_2.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如下圖，取△ABC的邊BC的三等分點D，連接AD並取中點E，連接BE並延長與AC相交於點F，那麼四邊形CDEF的面積是三角形ABC面積的【4/15 】。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>18.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>20_1.jpg 20_2.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>22_1.jpg 22_2.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如下圖，在三角形ABC中，BD：DC＝2：3，E是AD的中點。求陰影部份的面積是三角形ABC面積的【 3/8 】。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如圖，D是△ABC中BC邊上的一點，BC＝4CD，連接AD，E是AD的中點，連接BE並延長，交AC於點F，已知△ABC的面積112cm2，求四邊形CDEF  的面積【22】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">已知圖中三角形ABC的面積為8 cm2，AE＝ED，BD＝ 2/3BC，求：陰影部分的面積＝【3.2】cm2
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如下圖，在△ABC中，DC＝3BD，AE＝ED，若△ABC的面積是10cm2，則陰影部份的面積是【 30/7 】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>在△ABC中，DC＝3BD，DE＝EA，若△ABC的面積是2，則陰影部分面積＝【 6/7 】</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">D是BC上的一點，且BD＝3DC，E是AD上的一點，且AE＝2ED。已知△ABC的面積是60 cm2。求：四邊形CDEF的面積＝【9】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如圖所示，DE＝ 1/2AE，BD＝2DC，S△EBD＝5 cm2。求：三角形ABC的面積 ＝【45/2 】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>在△ABC中，DC：BC＝2：5，BO：OE＝4：1，那麼AE與EC的比＝【3:5】</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">△ABC的面積是12 cm2，且AE＝ 1/2EC，F是AD的中點，則：陰影部份的面積  ＝【5】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_1.jpg 2_2.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>四邊形</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">正方形ABCD的邊長28 cm2，F是BC的中點，AB的長是EB的4倍。連接AF、 CE，相交於G點。求：四邊形AGCD的面積＝【560】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">長方形ABCD的面積是2 cm2，EC＝2DE， F是DG的中點，陰影部分的面積＝【 5/12 】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">四邊形ABCD是邊長為12 cm的正方形，E、F分別是AB、BC的中點，AF與CE相交於G，則四邊形AGCD的面積＝【96】cm2。
+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_1.jpg 1_2.jpg</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_1.jpg 2_2.jpg</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -27176,7 +27440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -27212,6 +27476,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -27660,17 +27927,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H212"/>
+  <dimension ref="A1:H244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D184" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H212" sqref="H212"/>
+    <sheetView tabSelected="1" topLeftCell="D193" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G211" sqref="G211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="187.7109375" customWidth="1"/>
+    <col min="7" max="7" width="106.5703125" customWidth="1"/>
     <col min="8" max="8" width="60.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -33183,7 +33450,839 @@
         <v>231</v>
       </c>
       <c r="H212" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" ht="16.5">
+      <c r="A213" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C213" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D213" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E213" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F213" s="6">
+        <v>2</v>
+      </c>
+      <c r="G213" s="7" t="s">
         <v>236</v>
+      </c>
+      <c r="H213" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" ht="16.5">
+      <c r="A214" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C214" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D214" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E214" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F214" s="6">
+        <v>3</v>
+      </c>
+      <c r="G214" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="H214" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" ht="16.5">
+      <c r="A215" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C215" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D215" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E215" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F215" s="6">
+        <v>1</v>
+      </c>
+      <c r="G215" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="H215" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="16.5">
+      <c r="A216" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C216" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D216" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E216" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F216" s="6">
+        <v>2</v>
+      </c>
+      <c r="G216" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="H216" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" ht="16.5">
+      <c r="A217" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B217" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C217" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D217" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E217" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F217" s="6">
+        <v>3</v>
+      </c>
+      <c r="G217" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H217" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" ht="16.5">
+      <c r="A218" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C218" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D218" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E218" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F218" s="6">
+        <v>4</v>
+      </c>
+      <c r="G218" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="H218" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" ht="31.5">
+      <c r="A219" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C219" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D219" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E219" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F219" s="6">
+        <v>5</v>
+      </c>
+      <c r="G219" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="H219" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" ht="16.5">
+      <c r="A220" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C220" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D220" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E220" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F220" s="6">
+        <v>6</v>
+      </c>
+      <c r="G220" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="H220" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" ht="31.5">
+      <c r="A221" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C221" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D221" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E221" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F221" s="6">
+        <v>7</v>
+      </c>
+      <c r="G221" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="H221" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" ht="47.25">
+      <c r="A222" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B222" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C222" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D222" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E222" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F222" s="6">
+        <v>8</v>
+      </c>
+      <c r="G222" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="H222" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" ht="31.5">
+      <c r="A223" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B223" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C223" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D223" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E223" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F223" s="6">
+        <v>9</v>
+      </c>
+      <c r="G223" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="H223" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" ht="31.5">
+      <c r="A224" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B224" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C224" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D224" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E224" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F224" s="6">
+        <v>10</v>
+      </c>
+      <c r="G224" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="H224" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="31.5">
+      <c r="A225" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C225" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D225" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E225" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F225" s="6">
+        <v>11</v>
+      </c>
+      <c r="G225" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="H225" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" ht="47.25">
+      <c r="A226" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C226" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D226" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E226" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F226" s="6">
+        <v>12</v>
+      </c>
+      <c r="G226" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="H226" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" ht="47.25">
+      <c r="A227" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C227" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D227" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E227" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F227" s="6">
+        <v>13</v>
+      </c>
+      <c r="G227" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="H227" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" ht="31.5">
+      <c r="A228" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B228" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C228" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D228" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E228" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F228" s="6">
+        <v>14</v>
+      </c>
+      <c r="G228" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="H228" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" ht="47.25">
+      <c r="A229" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C229" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D229" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E229" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F229" s="6">
+        <v>15</v>
+      </c>
+      <c r="G229" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="H229" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="31.5">
+      <c r="A230" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C230" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D230" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E230" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F230" s="6">
+        <v>16</v>
+      </c>
+      <c r="G230" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="H230" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" ht="16.5">
+      <c r="A231" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B231" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C231" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D231" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E231" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F231" s="6">
+        <v>17</v>
+      </c>
+      <c r="G231" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="H231" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" ht="47.25">
+      <c r="A232" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B232" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C232" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D232" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E232" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F232" s="6">
+        <v>18</v>
+      </c>
+      <c r="G232" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="H232" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="31.5">
+      <c r="A233" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B233" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C233" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D233" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E233" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F233" s="6">
+        <v>19</v>
+      </c>
+      <c r="G233" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="H233" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" ht="47.25">
+      <c r="A234" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B234" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C234" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D234" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E234" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F234" s="6">
+        <v>20</v>
+      </c>
+      <c r="G234" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="H234" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" ht="31.5">
+      <c r="A235" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B235" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C235" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D235" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E235" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F235" s="6">
+        <v>21</v>
+      </c>
+      <c r="G235" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="H235" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" ht="31.5">
+      <c r="A236" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B236" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C236" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D236" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E236" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F236" s="6">
+        <v>22</v>
+      </c>
+      <c r="G236" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="H236" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" ht="16.5">
+      <c r="A237" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B237" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C237" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D237" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E237" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F237" s="6">
+        <v>23</v>
+      </c>
+      <c r="G237" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="H237" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" ht="47.25">
+      <c r="A238" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B238" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C238" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D238" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E238" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F238" s="6">
+        <v>24</v>
+      </c>
+      <c r="G238" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="H238" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" ht="31.5">
+      <c r="A239" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B239" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C239" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D239" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E239" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F239" s="6">
+        <v>25</v>
+      </c>
+      <c r="G239" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="H239" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" ht="16.5">
+      <c r="A240" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B240" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C240" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D240" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E240" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="F240" s="6">
+        <v>1</v>
+      </c>
+      <c r="G240" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="H240" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" ht="31.5">
+      <c r="A241" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B241" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C241" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D241" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E241" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="F241" s="6">
+        <v>2</v>
+      </c>
+      <c r="G241" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="H241" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" ht="47.25">
+      <c r="A242" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B242" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C242" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D242" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E242" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="F242" s="6">
+        <v>1</v>
+      </c>
+      <c r="G242" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="H242" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" ht="31.5">
+      <c r="A243" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B243" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C243" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D243" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E243" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="F243" s="6">
+        <v>2</v>
+      </c>
+      <c r="G243" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="H243" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" ht="47.25">
+      <c r="A244" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B244" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C244" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D244" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E244" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="F244" s="6">
+        <v>3</v>
+      </c>
+      <c r="G244" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="H244" s="6" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QDS Ver 0.1.8 : - Add class Question -Fix the problem that image not match the question
</commit_message>
<xml_diff>
--- a/database/盈虧問題v2.xlsx
+++ b/database/盈虧問題v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Question DataBase System\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDFED02-F7CE-4F09-9F39-F4AD9E9C414A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27274C3-372E-46CF-BA5D-80606834FC7E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="1830" windowWidth="10185" windowHeight="9795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12255" yWindow="1845" windowWidth="14505" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="299">
   <si>
     <r>
       <rPr>
@@ -27261,10 +27261,6 @@
   <si>
     <t xml:space="preserve">△ABC的面積是12 cm2，且AE＝ 1/2EC，F是AD的中點，則：陰影部份的面積  ＝【5】cm2。
 </t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>1_1.jpg 2_2.jpg</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -27929,8 +27925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D193" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G211" sqref="G211"/>
+    <sheetView tabSelected="1" topLeftCell="H192" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I201" sqref="I201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -27967,7 +27963,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5">
+    <row r="2" spans="1:8" ht="33">
       <c r="A2" s="6" t="s">
         <v>190</v>
       </c>
@@ -27993,7 +27989,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5">
+    <row r="3" spans="1:8" ht="33">
       <c r="A3" s="6" t="s">
         <v>190</v>
       </c>
@@ -28045,7 +28041,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.5">
+    <row r="5" spans="1:8" ht="33">
       <c r="A5" s="6" t="s">
         <v>190</v>
       </c>
@@ -28123,7 +28119,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5">
+    <row r="8" spans="1:8" ht="33">
       <c r="A8" s="6" t="s">
         <v>190</v>
       </c>
@@ -28149,7 +28145,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5">
+    <row r="9" spans="1:8" ht="33">
       <c r="A9" s="6" t="s">
         <v>190</v>
       </c>
@@ -28201,7 +28197,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.5">
+    <row r="11" spans="1:8" ht="33">
       <c r="A11" s="6" t="s">
         <v>190</v>
       </c>
@@ -28227,7 +28223,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.5">
+    <row r="12" spans="1:8" ht="33">
       <c r="A12" s="6" t="s">
         <v>190</v>
       </c>
@@ -28253,7 +28249,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.5">
+    <row r="13" spans="1:8" ht="33">
       <c r="A13" s="6" t="s">
         <v>190</v>
       </c>
@@ -28279,7 +28275,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16.5">
+    <row r="14" spans="1:8" ht="33">
       <c r="A14" s="6" t="s">
         <v>190</v>
       </c>
@@ -29189,7 +29185,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16.5">
+    <row r="49" spans="1:8" ht="33">
       <c r="A49" s="6" t="s">
         <v>190</v>
       </c>
@@ -29501,7 +29497,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="16.5">
+    <row r="61" spans="1:8" ht="33">
       <c r="A61" s="6" t="s">
         <v>190</v>
       </c>
@@ -29527,7 +29523,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="16.5">
+    <row r="62" spans="1:8" ht="33">
       <c r="A62" s="6" t="s">
         <v>190</v>
       </c>
@@ -30853,7 +30849,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="16.5">
+    <row r="113" spans="1:8" ht="33">
       <c r="A113" s="6" t="s">
         <v>190</v>
       </c>
@@ -30983,7 +30979,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="16.5">
+    <row r="118" spans="1:8" ht="33">
       <c r="A118" s="6" t="s">
         <v>190</v>
       </c>
@@ -31295,7 +31291,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="33">
+    <row r="130" spans="1:8" ht="49.5">
       <c r="A130" s="6" t="s">
         <v>190</v>
       </c>
@@ -31425,7 +31421,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="16.5">
+    <row r="135" spans="1:8" ht="33">
       <c r="A135" s="6" t="s">
         <v>190</v>
       </c>
@@ -31685,7 +31681,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="33">
+    <row r="145" spans="1:8" ht="49.5">
       <c r="A145" s="6" t="s">
         <v>190</v>
       </c>
@@ -31789,7 +31785,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="33">
+    <row r="149" spans="1:8" ht="49.5">
       <c r="A149" s="6" t="s">
         <v>190</v>
       </c>
@@ -34178,7 +34174,7 @@
         <v>291</v>
       </c>
       <c r="H240" s="6" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="241" spans="1:8" ht="31.5">
@@ -34221,16 +34217,16 @@
         <v>230</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F242" s="6">
         <v>1</v>
       </c>
       <c r="G242" s="14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H242" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="243" spans="1:8" ht="31.5">
@@ -34247,16 +34243,16 @@
         <v>230</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F243" s="6">
         <v>2</v>
       </c>
       <c r="G243" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H243" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="244" spans="1:8" ht="47.25">
@@ -34273,13 +34269,13 @@
         <v>230</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F244" s="6">
         <v>3</v>
       </c>
       <c r="G244" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H244" s="6" t="s">
         <v>241</v>

</xml_diff>

<commit_message>
Add Question stage3 : - Test make question after add question successful - Next : Add Back / MainMenu to switch into Make / Add(Edit) Question - Next : Image Add
</commit_message>
<xml_diff>
--- a/database/盈虧問題v2.xlsx
+++ b/database/盈虧問題v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Question DataBase System\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40953FD-8BEC-462E-BFAE-78718D8FF31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7428FF0-96C6-428A-8244-533FFBE8C572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="20205" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="300">
   <si>
     <t>第一層</t>
   </si>
@@ -858,9 +858,6 @@
 </t>
   </si>
   <si>
-    <t>5555</t>
-  </si>
-  <si>
     <t>NOIMAGE</t>
   </si>
   <si>
@@ -943,6 +940,14 @@
   </si>
   <si>
     <t>2_1.jpg 2_2.jpg</t>
+  </si>
+  <si>
+    <t>猜猜我再想什麼?【55555】</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>速寫課程中，構圖時需要先有個三角形，接著要注意動態、比例、構圖，請問一學期要交【200】張圖，才會過?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1351,13 +1356,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H245"/>
+  <dimension ref="A1:H246"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="H245" sqref="A245:H245"/>
+      <selection activeCell="P243" sqref="P243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1408,7 +1416,7 @@
         <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1434,7 +1442,7 @@
         <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1460,7 +1468,7 @@
         <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1486,7 +1494,7 @@
         <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1512,7 +1520,7 @@
         <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1538,7 +1546,7 @@
         <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1564,7 +1572,7 @@
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1590,7 +1598,7 @@
         <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1616,7 +1624,7 @@
         <v>35</v>
       </c>
       <c r="H10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1642,7 +1650,7 @@
         <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1668,7 +1676,7 @@
         <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1694,7 +1702,7 @@
         <v>38</v>
       </c>
       <c r="H13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1720,7 +1728,7 @@
         <v>39</v>
       </c>
       <c r="H14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1746,7 +1754,7 @@
         <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1772,7 +1780,7 @@
         <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1798,7 +1806,7 @@
         <v>42</v>
       </c>
       <c r="H17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1824,7 +1832,7 @@
         <v>43</v>
       </c>
       <c r="H18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1850,7 +1858,7 @@
         <v>44</v>
       </c>
       <c r="H19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1876,7 +1884,7 @@
         <v>45</v>
       </c>
       <c r="H20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1902,7 +1910,7 @@
         <v>46</v>
       </c>
       <c r="H21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1928,7 +1936,7 @@
         <v>47</v>
       </c>
       <c r="H22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1954,7 +1962,7 @@
         <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1980,7 +1988,7 @@
         <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2006,7 +2014,7 @@
         <v>50</v>
       </c>
       <c r="H25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2032,7 +2040,7 @@
         <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2058,7 +2066,7 @@
         <v>52</v>
       </c>
       <c r="H27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2084,7 +2092,7 @@
         <v>53</v>
       </c>
       <c r="H28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2110,7 +2118,7 @@
         <v>54</v>
       </c>
       <c r="H29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2136,7 +2144,7 @@
         <v>55</v>
       </c>
       <c r="H30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2162,7 +2170,7 @@
         <v>56</v>
       </c>
       <c r="H31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2188,7 +2196,7 @@
         <v>57</v>
       </c>
       <c r="H32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2214,7 +2222,7 @@
         <v>58</v>
       </c>
       <c r="H33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2240,7 +2248,7 @@
         <v>59</v>
       </c>
       <c r="H34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2266,7 +2274,7 @@
         <v>60</v>
       </c>
       <c r="H35" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2292,7 +2300,7 @@
         <v>61</v>
       </c>
       <c r="H36" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2318,7 +2326,7 @@
         <v>62</v>
       </c>
       <c r="H37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2344,7 +2352,7 @@
         <v>63</v>
       </c>
       <c r="H38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2370,7 +2378,7 @@
         <v>64</v>
       </c>
       <c r="H39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2396,7 +2404,7 @@
         <v>65</v>
       </c>
       <c r="H40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2422,7 +2430,7 @@
         <v>66</v>
       </c>
       <c r="H41" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2448,7 +2456,7 @@
         <v>67</v>
       </c>
       <c r="H42" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2474,7 +2482,7 @@
         <v>68</v>
       </c>
       <c r="H43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2500,7 +2508,7 @@
         <v>69</v>
       </c>
       <c r="H44" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2526,7 +2534,7 @@
         <v>70</v>
       </c>
       <c r="H45" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2552,7 +2560,7 @@
         <v>71</v>
       </c>
       <c r="H46" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2578,7 +2586,7 @@
         <v>72</v>
       </c>
       <c r="H47" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2604,7 +2612,7 @@
         <v>73</v>
       </c>
       <c r="H48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2630,7 +2638,7 @@
         <v>74</v>
       </c>
       <c r="H49" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2656,7 +2664,7 @@
         <v>75</v>
       </c>
       <c r="H50" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2682,7 +2690,7 @@
         <v>76</v>
       </c>
       <c r="H51" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2708,7 +2716,7 @@
         <v>77</v>
       </c>
       <c r="H52" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2734,7 +2742,7 @@
         <v>78</v>
       </c>
       <c r="H53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2760,7 +2768,7 @@
         <v>79</v>
       </c>
       <c r="H54" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2786,7 +2794,7 @@
         <v>80</v>
       </c>
       <c r="H55" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2812,7 +2820,7 @@
         <v>81</v>
       </c>
       <c r="H56" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2838,7 +2846,7 @@
         <v>82</v>
       </c>
       <c r="H57" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2864,7 +2872,7 @@
         <v>83</v>
       </c>
       <c r="H58" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2890,7 +2898,7 @@
         <v>84</v>
       </c>
       <c r="H59" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2916,7 +2924,7 @@
         <v>85</v>
       </c>
       <c r="H60" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2942,7 +2950,7 @@
         <v>86</v>
       </c>
       <c r="H61" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2968,7 +2976,7 @@
         <v>87</v>
       </c>
       <c r="H62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2994,7 +3002,7 @@
         <v>88</v>
       </c>
       <c r="H63" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3020,7 +3028,7 @@
         <v>89</v>
       </c>
       <c r="H64" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3046,7 +3054,7 @@
         <v>90</v>
       </c>
       <c r="H65" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3072,7 +3080,7 @@
         <v>91</v>
       </c>
       <c r="H66" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3098,7 +3106,7 @@
         <v>92</v>
       </c>
       <c r="H67" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3124,7 +3132,7 @@
         <v>93</v>
       </c>
       <c r="H68" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -3150,7 +3158,7 @@
         <v>94</v>
       </c>
       <c r="H69" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -3176,7 +3184,7 @@
         <v>95</v>
       </c>
       <c r="H70" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -3202,7 +3210,7 @@
         <v>96</v>
       </c>
       <c r="H71" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3228,7 +3236,7 @@
         <v>97</v>
       </c>
       <c r="H72" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3254,7 +3262,7 @@
         <v>98</v>
       </c>
       <c r="H73" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3280,7 +3288,7 @@
         <v>99</v>
       </c>
       <c r="H74" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3306,7 +3314,7 @@
         <v>100</v>
       </c>
       <c r="H75" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3332,7 +3340,7 @@
         <v>101</v>
       </c>
       <c r="H76" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3358,7 +3366,7 @@
         <v>102</v>
       </c>
       <c r="H77" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3384,7 +3392,7 @@
         <v>103</v>
       </c>
       <c r="H78" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3410,7 +3418,7 @@
         <v>104</v>
       </c>
       <c r="H79" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3436,7 +3444,7 @@
         <v>105</v>
       </c>
       <c r="H80" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3462,7 +3470,7 @@
         <v>106</v>
       </c>
       <c r="H81" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3488,7 +3496,7 @@
         <v>107</v>
       </c>
       <c r="H82" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3514,7 +3522,7 @@
         <v>108</v>
       </c>
       <c r="H83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3540,7 +3548,7 @@
         <v>109</v>
       </c>
       <c r="H84" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3566,7 +3574,7 @@
         <v>110</v>
       </c>
       <c r="H85" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3592,7 +3600,7 @@
         <v>111</v>
       </c>
       <c r="H86" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3618,7 +3626,7 @@
         <v>112</v>
       </c>
       <c r="H87" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3644,7 +3652,7 @@
         <v>113</v>
       </c>
       <c r="H88" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3670,7 +3678,7 @@
         <v>114</v>
       </c>
       <c r="H89" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3696,7 +3704,7 @@
         <v>115</v>
       </c>
       <c r="H90" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3722,7 +3730,7 @@
         <v>116</v>
       </c>
       <c r="H91" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3748,7 +3756,7 @@
         <v>117</v>
       </c>
       <c r="H92" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3774,7 +3782,7 @@
         <v>118</v>
       </c>
       <c r="H93" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3800,7 +3808,7 @@
         <v>119</v>
       </c>
       <c r="H94" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3826,7 +3834,7 @@
         <v>120</v>
       </c>
       <c r="H95" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3852,7 +3860,7 @@
         <v>121</v>
       </c>
       <c r="H96" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -3878,7 +3886,7 @@
         <v>122</v>
       </c>
       <c r="H97" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -3904,7 +3912,7 @@
         <v>123</v>
       </c>
       <c r="H98" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3930,7 +3938,7 @@
         <v>124</v>
       </c>
       <c r="H99" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3956,7 +3964,7 @@
         <v>125</v>
       </c>
       <c r="H100" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -3982,7 +3990,7 @@
         <v>126</v>
       </c>
       <c r="H101" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4008,7 +4016,7 @@
         <v>127</v>
       </c>
       <c r="H102" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4034,7 +4042,7 @@
         <v>128</v>
       </c>
       <c r="H103" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -4060,7 +4068,7 @@
         <v>129</v>
       </c>
       <c r="H104" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -4086,7 +4094,7 @@
         <v>130</v>
       </c>
       <c r="H105" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -4112,7 +4120,7 @@
         <v>131</v>
       </c>
       <c r="H106" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -4138,7 +4146,7 @@
         <v>132</v>
       </c>
       <c r="H107" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -4164,7 +4172,7 @@
         <v>133</v>
       </c>
       <c r="H108" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -4190,7 +4198,7 @@
         <v>134</v>
       </c>
       <c r="H109" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -4216,7 +4224,7 @@
         <v>135</v>
       </c>
       <c r="H110" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -4242,7 +4250,7 @@
         <v>136</v>
       </c>
       <c r="H111" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -4268,7 +4276,7 @@
         <v>137</v>
       </c>
       <c r="H112" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -4294,7 +4302,7 @@
         <v>138</v>
       </c>
       <c r="H113" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -4320,7 +4328,7 @@
         <v>139</v>
       </c>
       <c r="H114" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -4346,7 +4354,7 @@
         <v>140</v>
       </c>
       <c r="H115" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -4372,7 +4380,7 @@
         <v>141</v>
       </c>
       <c r="H116" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -4398,7 +4406,7 @@
         <v>142</v>
       </c>
       <c r="H117" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -4424,7 +4432,7 @@
         <v>143</v>
       </c>
       <c r="H118" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -4450,7 +4458,7 @@
         <v>144</v>
       </c>
       <c r="H119" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -4476,7 +4484,7 @@
         <v>145</v>
       </c>
       <c r="H120" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -4502,7 +4510,7 @@
         <v>146</v>
       </c>
       <c r="H121" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -4528,7 +4536,7 @@
         <v>147</v>
       </c>
       <c r="H122" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -4554,7 +4562,7 @@
         <v>148</v>
       </c>
       <c r="H123" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -4580,7 +4588,7 @@
         <v>149</v>
       </c>
       <c r="H124" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -4606,7 +4614,7 @@
         <v>150</v>
       </c>
       <c r="H125" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -4632,7 +4640,7 @@
         <v>151</v>
       </c>
       <c r="H126" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -4658,7 +4666,7 @@
         <v>152</v>
       </c>
       <c r="H127" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -4684,7 +4692,7 @@
         <v>153</v>
       </c>
       <c r="H128" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -4710,7 +4718,7 @@
         <v>154</v>
       </c>
       <c r="H129" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -4736,7 +4744,7 @@
         <v>155</v>
       </c>
       <c r="H130" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -4762,7 +4770,7 @@
         <v>156</v>
       </c>
       <c r="H131" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -4788,7 +4796,7 @@
         <v>157</v>
       </c>
       <c r="H132" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -4814,7 +4822,7 @@
         <v>158</v>
       </c>
       <c r="H133" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -4840,7 +4848,7 @@
         <v>159</v>
       </c>
       <c r="H134" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -4866,7 +4874,7 @@
         <v>160</v>
       </c>
       <c r="H135" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -4892,7 +4900,7 @@
         <v>161</v>
       </c>
       <c r="H136" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -4918,7 +4926,7 @@
         <v>162</v>
       </c>
       <c r="H137" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -4944,7 +4952,7 @@
         <v>163</v>
       </c>
       <c r="H138" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -4970,7 +4978,7 @@
         <v>164</v>
       </c>
       <c r="H139" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -4996,7 +5004,7 @@
         <v>165</v>
       </c>
       <c r="H140" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -5022,7 +5030,7 @@
         <v>166</v>
       </c>
       <c r="H141" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -5048,7 +5056,7 @@
         <v>167</v>
       </c>
       <c r="H142" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -5074,7 +5082,7 @@
         <v>168</v>
       </c>
       <c r="H143" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -5100,7 +5108,7 @@
         <v>169</v>
       </c>
       <c r="H144" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -5126,7 +5134,7 @@
         <v>170</v>
       </c>
       <c r="H145" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -5152,7 +5160,7 @@
         <v>171</v>
       </c>
       <c r="H146" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -5178,7 +5186,7 @@
         <v>172</v>
       </c>
       <c r="H147" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -5204,7 +5212,7 @@
         <v>173</v>
       </c>
       <c r="H148" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -5230,7 +5238,7 @@
         <v>174</v>
       </c>
       <c r="H149" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -5256,7 +5264,7 @@
         <v>175</v>
       </c>
       <c r="H150" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -5282,7 +5290,7 @@
         <v>176</v>
       </c>
       <c r="H151" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -5308,7 +5316,7 @@
         <v>177</v>
       </c>
       <c r="H152" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -5334,7 +5342,7 @@
         <v>178</v>
       </c>
       <c r="H153" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -5360,7 +5368,7 @@
         <v>179</v>
       </c>
       <c r="H154" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -5386,7 +5394,7 @@
         <v>180</v>
       </c>
       <c r="H155" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -5412,7 +5420,7 @@
         <v>181</v>
       </c>
       <c r="H156" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -5438,7 +5446,7 @@
         <v>182</v>
       </c>
       <c r="H157" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -5464,7 +5472,7 @@
         <v>183</v>
       </c>
       <c r="H158" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -5490,7 +5498,7 @@
         <v>184</v>
       </c>
       <c r="H159" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -5516,7 +5524,7 @@
         <v>185</v>
       </c>
       <c r="H160" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -5542,7 +5550,7 @@
         <v>186</v>
       </c>
       <c r="H161" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -5568,7 +5576,7 @@
         <v>187</v>
       </c>
       <c r="H162" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -5594,7 +5602,7 @@
         <v>188</v>
       </c>
       <c r="H163" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -5620,7 +5628,7 @@
         <v>189</v>
       </c>
       <c r="H164" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -5646,7 +5654,7 @@
         <v>190</v>
       </c>
       <c r="H165" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -5672,7 +5680,7 @@
         <v>191</v>
       </c>
       <c r="H166" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -5698,7 +5706,7 @@
         <v>192</v>
       </c>
       <c r="H167" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -5724,7 +5732,7 @@
         <v>193</v>
       </c>
       <c r="H168" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -5750,7 +5758,7 @@
         <v>194</v>
       </c>
       <c r="H169" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -5776,7 +5784,7 @@
         <v>195</v>
       </c>
       <c r="H170" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -5802,7 +5810,7 @@
         <v>196</v>
       </c>
       <c r="H171" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -5828,7 +5836,7 @@
         <v>197</v>
       </c>
       <c r="H172" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -5854,7 +5862,7 @@
         <v>198</v>
       </c>
       <c r="H173" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -5880,7 +5888,7 @@
         <v>199</v>
       </c>
       <c r="H174" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -5906,7 +5914,7 @@
         <v>200</v>
       </c>
       <c r="H175" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -5932,7 +5940,7 @@
         <v>201</v>
       </c>
       <c r="H176" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -5958,7 +5966,7 @@
         <v>202</v>
       </c>
       <c r="H177" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -5984,7 +5992,7 @@
         <v>203</v>
       </c>
       <c r="H178" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -6010,7 +6018,7 @@
         <v>204</v>
       </c>
       <c r="H179" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -6036,7 +6044,7 @@
         <v>205</v>
       </c>
       <c r="H180" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -6062,7 +6070,7 @@
         <v>206</v>
       </c>
       <c r="H181" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -6088,7 +6096,7 @@
         <v>207</v>
       </c>
       <c r="H182" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -6114,7 +6122,7 @@
         <v>208</v>
       </c>
       <c r="H183" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -6140,7 +6148,7 @@
         <v>209</v>
       </c>
       <c r="H184" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -6166,7 +6174,7 @@
         <v>210</v>
       </c>
       <c r="H185" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
@@ -6192,7 +6200,7 @@
         <v>211</v>
       </c>
       <c r="H186" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -6218,7 +6226,7 @@
         <v>212</v>
       </c>
       <c r="H187" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -6244,7 +6252,7 @@
         <v>213</v>
       </c>
       <c r="H188" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
@@ -6270,7 +6278,7 @@
         <v>214</v>
       </c>
       <c r="H189" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -6296,7 +6304,7 @@
         <v>215</v>
       </c>
       <c r="H190" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
@@ -6322,7 +6330,7 @@
         <v>216</v>
       </c>
       <c r="H191" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
@@ -6348,7 +6356,7 @@
         <v>217</v>
       </c>
       <c r="H192" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -6374,7 +6382,7 @@
         <v>218</v>
       </c>
       <c r="H193" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -6400,7 +6408,7 @@
         <v>219</v>
       </c>
       <c r="H194" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -6426,7 +6434,7 @@
         <v>220</v>
       </c>
       <c r="H195" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -6452,7 +6460,7 @@
         <v>221</v>
       </c>
       <c r="H196" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -6478,7 +6486,7 @@
         <v>222</v>
       </c>
       <c r="H197" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
@@ -6504,7 +6512,7 @@
         <v>223</v>
       </c>
       <c r="H198" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -6530,7 +6538,7 @@
         <v>224</v>
       </c>
       <c r="H199" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
@@ -6556,7 +6564,7 @@
         <v>225</v>
       </c>
       <c r="H200" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
@@ -6582,7 +6590,7 @@
         <v>226</v>
       </c>
       <c r="H201" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
@@ -6608,7 +6616,7 @@
         <v>227</v>
       </c>
       <c r="H202" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
@@ -6634,7 +6642,7 @@
         <v>228</v>
       </c>
       <c r="H203" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
@@ -6660,7 +6668,7 @@
         <v>229</v>
       </c>
       <c r="H204" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
@@ -6686,7 +6694,7 @@
         <v>230</v>
       </c>
       <c r="H205" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
@@ -6712,7 +6720,7 @@
         <v>231</v>
       </c>
       <c r="H206" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
@@ -6738,7 +6746,7 @@
         <v>232</v>
       </c>
       <c r="H207" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
@@ -6764,7 +6772,7 @@
         <v>233</v>
       </c>
       <c r="H208" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
@@ -6790,7 +6798,7 @@
         <v>234</v>
       </c>
       <c r="H209" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
@@ -6816,7 +6824,7 @@
         <v>235</v>
       </c>
       <c r="H210" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
@@ -6842,7 +6850,7 @@
         <v>236</v>
       </c>
       <c r="H211" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -6868,7 +6876,7 @@
         <v>237</v>
       </c>
       <c r="H212" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -6894,7 +6902,7 @@
         <v>238</v>
       </c>
       <c r="H213" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -6920,7 +6928,7 @@
         <v>239</v>
       </c>
       <c r="H214" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
@@ -6946,7 +6954,7 @@
         <v>240</v>
       </c>
       <c r="H215" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
@@ -6972,7 +6980,7 @@
         <v>241</v>
       </c>
       <c r="H216" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -6998,7 +7006,7 @@
         <v>242</v>
       </c>
       <c r="H217" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -7024,7 +7032,7 @@
         <v>243</v>
       </c>
       <c r="H218" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -7050,7 +7058,7 @@
         <v>244</v>
       </c>
       <c r="H219" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -7076,7 +7084,7 @@
         <v>245</v>
       </c>
       <c r="H220" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -7102,7 +7110,7 @@
         <v>246</v>
       </c>
       <c r="H221" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -7128,7 +7136,7 @@
         <v>247</v>
       </c>
       <c r="H222" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -7154,7 +7162,7 @@
         <v>248</v>
       </c>
       <c r="H223" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -7180,7 +7188,7 @@
         <v>249</v>
       </c>
       <c r="H224" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -7206,7 +7214,7 @@
         <v>250</v>
       </c>
       <c r="H225" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
@@ -7232,7 +7240,7 @@
         <v>251</v>
       </c>
       <c r="H226" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
@@ -7258,7 +7266,7 @@
         <v>252</v>
       </c>
       <c r="H227" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
@@ -7284,7 +7292,7 @@
         <v>253</v>
       </c>
       <c r="H228" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -7310,7 +7318,7 @@
         <v>254</v>
       </c>
       <c r="H229" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
@@ -7336,7 +7344,7 @@
         <v>255</v>
       </c>
       <c r="H230" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
@@ -7362,7 +7370,7 @@
         <v>256</v>
       </c>
       <c r="H231" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
@@ -7388,7 +7396,7 @@
         <v>257</v>
       </c>
       <c r="H232" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
@@ -7414,7 +7422,7 @@
         <v>258</v>
       </c>
       <c r="H233" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
@@ -7440,7 +7448,7 @@
         <v>259</v>
       </c>
       <c r="H234" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
@@ -7466,7 +7474,7 @@
         <v>260</v>
       </c>
       <c r="H235" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
@@ -7492,7 +7500,7 @@
         <v>261</v>
       </c>
       <c r="H236" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
@@ -7518,7 +7526,7 @@
         <v>262</v>
       </c>
       <c r="H237" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
@@ -7544,7 +7552,7 @@
         <v>263</v>
       </c>
       <c r="H238" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
@@ -7570,7 +7578,7 @@
         <v>264</v>
       </c>
       <c r="H239" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
@@ -7596,7 +7604,7 @@
         <v>265</v>
       </c>
       <c r="H240" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
@@ -7622,7 +7630,7 @@
         <v>266</v>
       </c>
       <c r="H241" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
@@ -7648,7 +7656,7 @@
         <v>267</v>
       </c>
       <c r="H242" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
@@ -7674,7 +7682,7 @@
         <v>268</v>
       </c>
       <c r="H243" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
@@ -7700,7 +7708,7 @@
         <v>269</v>
       </c>
       <c r="H244" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
@@ -7723,10 +7731,36 @@
         <v>4</v>
       </c>
       <c r="G245" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="H245" t="s">
-        <v>271</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>8</v>
+      </c>
+      <c r="B246" t="s">
+        <v>9</v>
+      </c>
+      <c r="C246" t="s">
+        <v>10</v>
+      </c>
+      <c r="D246" t="s">
+        <v>12</v>
+      </c>
+      <c r="E246" t="s">
+        <v>25</v>
+      </c>
+      <c r="F246">
+        <v>5</v>
+      </c>
+      <c r="G246" t="s">
+        <v>299</v>
+      </c>
+      <c r="H246" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QDS Ver 0.3.2 image will resize to max size (256, 256), and keep width and height ratio
</commit_message>
<xml_diff>
--- a/database/盈虧問題v2.xlsx
+++ b/database/盈虧問題v2.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H260"/>
+  <dimension ref="A1:H250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10407,16 +10407,14 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>四邊形</t>
+          <t>胖子</t>
         </is>
       </c>
       <c r="F249" t="n">
-        <v>3</v>
-      </c>
-      <c r="G249" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="G249" t="n">
+        <v>123</v>
       </c>
       <c r="H249" t="inlineStr">
         <is>
@@ -10451,416 +10449,16 @@
         </is>
       </c>
       <c r="F250" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>165165opfjwieojfiowejfpowejmfol;mwel;'fwe+6</t>
+          <t>123456</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>4_1.jpg 4_2.png 4_3.jpg 4_4.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B251" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C251" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D251" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E251" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F251" t="n">
-        <v>5</v>
-      </c>
-      <c r="G251" t="inlineStr">
-        <is>
-          <t>45698498</t>
-        </is>
-      </c>
-      <c r="H251" t="inlineStr">
-        <is>
-          <t>5.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B252" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C252" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D252" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E252" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F252" t="n">
-        <v>6</v>
-      </c>
-      <c r="G252" t="inlineStr">
-        <is>
-          <t>526+++6</t>
-        </is>
-      </c>
-      <c r="H252" t="inlineStr">
-        <is>
-          <t>6.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B253" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C253" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D253" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E253" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F253" t="n">
-        <v>7</v>
-      </c>
-      <c r="G253" t="inlineStr">
-        <is>
-          <t>89+4894123198</t>
-        </is>
-      </c>
-      <c r="H253" t="inlineStr">
-        <is>
-          <t>7.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B254" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C254" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D254" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E254" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F254" t="n">
-        <v>8</v>
-      </c>
-      <c r="G254" t="inlineStr">
-        <is>
-          <t>16123549789</t>
-        </is>
-      </c>
-      <c r="H254" t="inlineStr">
-        <is>
-          <t>8_1.png 8_2.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B255" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C255" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D255" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E255" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F255" t="n">
-        <v>9</v>
-      </c>
-      <c r="G255" t="inlineStr">
-        <is>
-          <t>14245277278</t>
-        </is>
-      </c>
-      <c r="H255" t="inlineStr">
-        <is>
-          <t>9_1.png 9_2.jpg 9_3.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B256" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C256" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D256" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E256" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F256" t="n">
-        <v>10</v>
-      </c>
-      <c r="G256" t="inlineStr">
-        <is>
-          <t>527278278</t>
-        </is>
-      </c>
-      <c r="H256" t="inlineStr">
-        <is>
-          <t>10_1.png 10_2.jpg 10_3.jpg 10_4.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B257" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C257" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D257" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E257" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F257" t="n">
-        <v>11</v>
-      </c>
-      <c r="G257" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="H257" t="inlineStr">
-        <is>
-          <t>11.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B258" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C258" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D258" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E258" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F258" t="n">
-        <v>12</v>
-      </c>
-      <c r="G258" t="inlineStr">
-        <is>
-          <t>789456123456789</t>
-        </is>
-      </c>
-      <c r="H258" t="inlineStr">
-        <is>
-          <t>12_1.jpg 12_2.jpg 12_3.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B259" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C259" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D259" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E259" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F259" t="n">
-        <v>13</v>
-      </c>
-      <c r="G259" t="inlineStr">
-        <is>
-          <t>13131313345768978</t>
-        </is>
-      </c>
-      <c r="H259" t="inlineStr">
-        <is>
-          <t>13_1.png 13_2.jpg 13_3.jpg 13_4.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="inlineStr">
-        <is>
-          <t>數學</t>
-        </is>
-      </c>
-      <c r="B260" t="inlineStr">
-        <is>
-          <t>應用題</t>
-        </is>
-      </c>
-      <c r="C260" t="inlineStr">
-        <is>
-          <t>典型應用題</t>
-        </is>
-      </c>
-      <c r="D260" t="inlineStr">
-        <is>
-          <t>燕尾定理</t>
-        </is>
-      </c>
-      <c r="E260" t="inlineStr">
-        <is>
-          <t>四邊形</t>
-        </is>
-      </c>
-      <c r="F260" t="n">
-        <v>14</v>
-      </c>
-      <c r="G260" t="inlineStr">
-        <is>
-          <t>123459789</t>
-        </is>
-      </c>
-      <c r="H260" t="inlineStr">
-        <is>
-          <t>14_1.jpg 14_2.jpg 14_3.jpg</t>
+          <t>3.png</t>
         </is>
       </c>
     </row>

</xml_diff>